<commit_message>
Sube Archivos con Pruebas OK!
</commit_message>
<xml_diff>
--- a/data/Favorites_WEAP.xlsx
+++ b/data/Favorites_WEAP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aimee\Desktop\Github\WEAPMODFLOW_LP_Calibration\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E0F01C-9906-44E6-ADC0-5A0A6C4BBDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970BD88C-0325-43B9-B7D0-E5692276C227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Favorites" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -230,13 +230,7 @@
     <t>\Precipitation_SC_AGR</t>
   </si>
   <si>
-    <t>\Pozos - Observados</t>
-  </si>
-  <si>
     <t>Simulated_wells</t>
-  </si>
-  <si>
-    <t>Observated_wells</t>
   </si>
 </sst>
 </file>
@@ -647,16 +641,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J133"/>
+  <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.53125" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" style="1" bestFit="1" customWidth="1"/>
@@ -946,29 +940,29 @@
         <v>35</v>
       </c>
       <c r="D16" s="4" t="str">
-        <f t="shared" ref="D16:D31" si="1">CONCATENATE(B16,C16)</f>
+        <f t="shared" ref="D16:D30" si="1">CONCATENATE(B16,C16)</f>
         <v>MODFLOW y Acuiferos\Pozos - Simulados</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="D17" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\Pozos - Observados</v>
+        <v>MODFLOW y Acuiferos\SHAC - L01</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
@@ -979,14 +973,14 @@
         <v>34</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - L01</v>
+        <v>MODFLOW y Acuiferos\SHAC - L02</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
@@ -997,14 +991,14 @@
         <v>34</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - L02</v>
+        <v>MODFLOW y Acuiferos\SHAC - L05</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
@@ -1015,14 +1009,14 @@
         <v>34</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - L05</v>
+        <v>MODFLOW y Acuiferos\SHAC - L06</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
@@ -1033,14 +1027,14 @@
         <v>34</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - L06</v>
+        <v>MODFLOW y Acuiferos\SHAC - L09</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
@@ -1051,14 +1045,14 @@
         <v>34</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - L09</v>
+        <v>MODFLOW y Acuiferos\SHAC - L10</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
@@ -1069,14 +1063,14 @@
         <v>34</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - L10</v>
+        <v>MODFLOW y Acuiferos\SHAC - L12</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
@@ -1087,17 +1081,17 @@
         <v>34</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - L12</v>
+        <v>MODFLOW y Acuiferos\SHAC - P01</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>2</v>
       </c>
@@ -1105,15 +1099,18 @@
         <v>34</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D25" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - P01</v>
+        <v>MODFLOW y Acuiferos\SHAC - P02</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="J25"/>
     </row>
     <row r="26" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
@@ -1123,14 +1120,14 @@
         <v>34</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - P02</v>
+        <v>MODFLOW y Acuiferos\SHAC - P03</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G26"/>
       <c r="H26"/>
@@ -1144,14 +1141,14 @@
         <v>34</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - P03</v>
+        <v>MODFLOW y Acuiferos\SHAC - P07</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G27"/>
       <c r="H27"/>
@@ -1165,14 +1162,14 @@
         <v>34</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - P07</v>
+        <v>MODFLOW y Acuiferos\SHAC - P08-v1</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G28"/>
       <c r="H28"/>
@@ -1186,14 +1183,14 @@
         <v>34</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - P08-v1</v>
+        <v>MODFLOW y Acuiferos\SHAC - P08-v2</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G29"/>
       <c r="H29"/>
@@ -1201,42 +1198,31 @@
     </row>
     <row r="30" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D30" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>MODFLOW y Acuiferos\SHAC - P08-v2</v>
+        <v>Precipitation\Precipitation_SC_AGR</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
       <c r="J30"/>
     </row>
     <row r="31" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="4">
-        <v>3</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Precipitation\Precipitation_SC_AGR</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
       <c r="G31"/>
       <c r="H31"/>
       <c r="J31"/>
@@ -1917,7 +1903,6 @@
       <c r="C99" s="5"/>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
-      <c r="G99"/>
       <c r="H99"/>
       <c r="J99"/>
     </row>
@@ -1981,7 +1966,6 @@
       <c r="C106" s="5"/>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
-      <c r="H106"/>
       <c r="J106"/>
     </row>
     <row r="107" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1990,6 +1974,8 @@
       <c r="C107" s="5"/>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
+      <c r="G107"/>
+      <c r="H107"/>
       <c r="J107"/>
     </row>
     <row r="108" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -2242,16 +2228,6 @@
       <c r="H132"/>
       <c r="J132"/>
     </row>
-    <row r="133" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A133" s="4"/>
-      <c r="B133" s="4"/>
-      <c r="C133" s="5"/>
-      <c r="D133" s="4"/>
-      <c r="E133" s="4"/>
-      <c r="G133"/>
-      <c r="H133"/>
-      <c r="J133"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>